<commit_message>
Definición de los usuarios
Entrada en bitácora y definición de los usuarios de la aplicación.
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -71,9 +71,6 @@
     <t>App Definition</t>
   </si>
   <si>
-    <t>Users/Similar Systems</t>
-  </si>
-  <si>
     <t>12 mins (11:11 - 11:23)</t>
   </si>
   <si>
@@ -81,6 +78,18 @@
   </si>
   <si>
     <t>Goals</t>
+  </si>
+  <si>
+    <t>Similar Systems</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>18 mins (11:32 - 11:50)</t>
+  </si>
+  <si>
+    <t>Nice, the definition of possible users was an interesting task.</t>
   </si>
 </sst>
 </file>
@@ -116,10 +125,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +418,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -457,34 +472,53 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>43522</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revisión de la defición de la aplicación y del plan te investigación. Registro en bitácora
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauriciorodriguez/Documents/GitHub/HCI-Team4-Workspace/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EF7DB7-5F4D-454C-AA0F-AE684CEDDBC1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="2100" windowWidth="20740" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,18 +15,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -96,12 +92,33 @@
   </si>
   <si>
     <t>Ok, the research was made before so it was a pretty boring task</t>
+  </si>
+  <si>
+    <t>App requests</t>
+  </si>
+  <si>
+    <t>Interview</t>
+  </si>
+  <si>
+    <t>2 hours (05:30 - 07:00)</t>
+  </si>
+  <si>
+    <t>Requeriments</t>
+  </si>
+  <si>
+    <t>1.5 hours (3:30 - 05:00)</t>
+  </si>
+  <si>
+    <t>Nice, I made a small talk with different Stakeholders</t>
+  </si>
+  <si>
+    <t>Ok, I made progress in the requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,24 +437,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43516</v>
       </c>
@@ -477,7 +494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43522</v>
       </c>
@@ -497,7 +514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -511,7 +528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -523,6 +540,46 @@
       </c>
       <c r="F5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43521</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perfiles, personas y escenarios
Se definieron las personas para el sistema que se desarrollará.
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>Ok, the research was made before so it was a pretty boring task</t>
+  </si>
+  <si>
+    <t>1hr 7min (20:36 - 21:43)</t>
+  </si>
+  <si>
+    <t>Profiles, Personas and scenarios</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Pleased, identifying the profile of possible users was a really interesting and pleasing task</t>
   </si>
 </sst>
 </file>
@@ -131,15 +143,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -478,13 +493,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>43522</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
@@ -498,9 +513,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="3"/>
       <c r="D4" t="s">
         <v>17</v>
       </c>
@@ -512,9 +527,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
       <c r="D5" t="s">
         <v>16</v>
       </c>
@@ -523,13 +538,29 @@
       </c>
       <c r="F5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corregí error de bitacora
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE49C52-09E4-4E2C-9E4F-813A7E4ABC4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A79B52-9CA0-4DE0-813E-251199414645}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:I17"/>
+      <selection activeCell="A6" sqref="A6:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,63 +554,63 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>43521</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>43522</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>43522</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificaciones a la bitácora
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25035A4B-1584-4AFA-87ED-23746540DB18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6776861-2FC6-466D-B31A-A74E47F0D0D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Actividades y satisfacción" sheetId="1" r:id="rId1"/>
+    <sheet name="Metricas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -155,6 +156,72 @@
   </si>
   <si>
     <t>What I learned?</t>
+  </si>
+  <si>
+    <t>Dificulty</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>30 mins (8:00 - 8:30)</t>
+  </si>
+  <si>
+    <t>Nice, too easy, we had all the info</t>
+  </si>
+  <si>
+    <t>Having the information is easier to make a presentation and takes less time</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>Promedio de estado de ánimo</t>
+  </si>
+  <si>
+    <t>Contribuciónes del equipo</t>
+  </si>
+  <si>
+    <t>Velocidad del equipo</t>
+  </si>
+  <si>
+    <t>Week 0</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Medicion de tiempos resultares semanales.</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
 </sst>
 </file>
@@ -190,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,6 +266,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,24 +550,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G11"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="75.28515625" customWidth="1"/>
-    <col min="7" max="7" width="48.140625" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="71" customWidth="1"/>
+    <col min="8" max="8" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -505,22 +576,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43516</v>
       </c>
@@ -528,67 +602,75 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43522</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43521</v>
       </c>
@@ -596,19 +678,22 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43522</v>
       </c>
@@ -616,19 +701,22 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43522</v>
       </c>
@@ -636,19 +724,22 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43522</v>
       </c>
@@ -656,19 +747,22 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43523</v>
       </c>
@@ -676,24 +770,253 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43523</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:D6"/>
     <mergeCell ref="C4:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDE2EF5-25AD-47C4-A52A-B3A972286807}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Registro de tareas acordadas en la bitácora
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6776861-2FC6-466D-B31A-A74E47F0D0D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47310B13-C251-42B8-A54F-0FF8A33CE62E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Actividades y satisfacción" sheetId="1" r:id="rId1"/>
-    <sheet name="Metricas" sheetId="2" r:id="rId2"/>
+    <sheet name="Actividades realizadas" sheetId="1" r:id="rId1"/>
+    <sheet name="Actividades definidas" sheetId="3" r:id="rId2"/>
+    <sheet name="Metricas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -222,6 +223,33 @@
   </si>
   <si>
     <t>Person</t>
+  </si>
+  <si>
+    <t>1.- Definición de la aplicación</t>
+  </si>
+  <si>
+    <t>2.- Plan de investigación</t>
+  </si>
+  <si>
+    <t>3.- Calendario de actividades</t>
+  </si>
+  <si>
+    <t>4.- Perfiles, personas, escenarios</t>
+  </si>
+  <si>
+    <t>Mauricio/Kirbey</t>
+  </si>
+  <si>
+    <t>5.- Definición de requerimientos</t>
+  </si>
+  <si>
+    <t>Edwin/Jorge</t>
+  </si>
+  <si>
+    <t>6.- Presentación</t>
+  </si>
+  <si>
+    <t>7.- Revisiónes</t>
   </si>
 </sst>
 </file>
@@ -553,7 +581,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,6 +851,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16224AAD-DAF0-41BA-8CFF-52F0C4E8E299}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDE2EF5-25AD-47C4-A52A-B3A972286807}">
   <dimension ref="A1:F26"/>
   <sheetViews>

</xml_diff>

<commit_message>
Entrada a la bitácora sobre Mesa redonda
Se agregó en la bitácora la información sobre los tiempos de la mesa redonda.
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauriciorodriguez/Documents/GitHub/HCI-Team4-Workspace/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="1800" yWindow="460" windowWidth="27000" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades realizadas" sheetId="1" r:id="rId1"/>
@@ -16,18 +21,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
   <si>
     <t>Date</t>
   </si>
@@ -267,12 +272,24 @@
   </si>
   <si>
     <t xml:space="preserve">Ok, the perspective's interviewed was interesting and gave ideas about the future the app </t>
+  </si>
+  <si>
+    <t>RoundTable</t>
+  </si>
+  <si>
+    <t>1hr 30 min (19:00 - 20:30)</t>
+  </si>
+  <si>
+    <t>Great, it was interesting to gather new points of view and the activity was enjoyable.</t>
+  </si>
+  <si>
+    <t>Some other reasons that causes people to feel depressed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -300,11 +317,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -313,7 +330,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -321,17 +338,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -341,7 +358,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -349,12 +366,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -363,31 +380,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -395,23 +412,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -436,6 +453,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -454,8 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,27 +753,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I14"/>
+  <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="78.28515625" customWidth="1"/>
-    <col min="9" max="9" width="68.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="78.33203125" customWidth="1"/>
+    <col min="9" max="9" width="68.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -782,7 +799,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="14">
         <v>43516</v>
       </c>
@@ -806,17 +823,17 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="18">
         <v>43522</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -830,11 +847,11 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="17"/>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
@@ -846,11 +863,11 @@
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="17"/>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
@@ -862,7 +879,7 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="14">
         <v>43521</v>
       </c>
@@ -886,7 +903,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="14">
         <v>43522</v>
       </c>
@@ -910,31 +927,31 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="14">
         <v>43522</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="17" t="s">
         <v>77</v>
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="14">
         <v>43522</v>
       </c>
@@ -958,7 +975,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="14">
         <v>43522</v>
       </c>
@@ -982,7 +999,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="14">
         <v>43523</v>
       </c>
@@ -1006,7 +1023,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>43523</v>
       </c>
@@ -1032,27 +1049,53 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="16">
         <v>43529</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="17" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="16">
+        <v>43512</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1074,13 +1117,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1091,7 +1134,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>65</v>
       </c>
@@ -1102,7 +1145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>66</v>
       </c>
@@ -1113,7 +1156,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>67</v>
       </c>
@@ -1124,7 +1167,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
@@ -1135,7 +1178,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
@@ -1146,7 +1189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>72</v>
       </c>
@@ -1157,7 +1200,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>73</v>
       </c>
@@ -1182,20 +1225,20 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
@@ -1215,7 +1258,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>44</v>
       </c>
@@ -1227,7 +1270,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
@@ -1239,7 +1282,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>50</v>
       </c>
@@ -1251,18 +1294,18 @@
       <c r="F6" s="9"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    <row r="7" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>64</v>
       </c>
@@ -1282,7 +1325,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1292,7 +1335,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1302,7 +1345,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>62</v>
       </c>
@@ -1312,7 +1355,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1322,18 +1365,18 @@
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+    <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>64</v>
       </c>
@@ -1353,7 +1396,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
@@ -1363,7 +1406,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
@@ -1373,7 +1416,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
         <v>62</v>
       </c>
@@ -1383,7 +1426,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
@@ -1393,18 +1436,18 @@
       <c r="F20" s="9"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+    <row r="21" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
@@ -1424,7 +1467,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>4</v>
       </c>
@@ -1434,7 +1477,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>33</v>
       </c>
@@ -1444,7 +1487,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
         <v>62</v>
       </c>
@@ -1454,7 +1497,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>11</v>
       </c>

</xml_diff>